<commit_message>
pequennas correcciones en el sistema
</commit_message>
<xml_diff>
--- a/src/informesGenerados/ResumenFGR.xlsx
+++ b/src/informesGenerados/ResumenFGR.xlsx
@@ -1119,7 +1119,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -1128,10 +1128,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2</c:v>
@@ -3644,7 +3644,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>2020: 38 hechos</c:v>
+            <c:v>2020: 34 hechos</c:v>
           </c:tx>
           <c:dLbls>
             <c:spPr>
@@ -3787,7 +3787,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>3</c:v>
@@ -3799,7 +3799,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1</c:v>
@@ -4086,7 +4086,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>2020: 43 hechos</c:v>
+            <c:v>2020: 38 hechos</c:v>
           </c:tx>
           <c:dLbls>
             <c:spPr>
@@ -4229,7 +4229,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
@@ -4241,7 +4241,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1</c:v>
@@ -5291,11 +5291,11 @@
         <v>61</v>
       </c>
       <c r="C2" s="4">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D2" s="5">
         <f ca="1">B2+C2</f>
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" ht="26.25" customHeight="true">
@@ -5323,11 +5323,11 @@
       </c>
       <c r="C4" s="3" t="str">
         <f ca="1">IF(C3&gt;C2,(C3-C2)&amp;" más",IF(C2&gt;C3,(C2-C3)&amp;" menos","Igual"))</f>
-        <v>17 menos</v>
+        <v>13 menos</v>
       </c>
       <c r="D4" s="5" t="str">
         <f ca="1">IF(D3&gt;D2,(D3-D2)&amp;" más",IF(D2&gt;D3,(D2-D3)&amp;" menos","Igual"))</f>
-        <v>3 menos</v>
+        <v>1 más</v>
       </c>
     </row>
     <row r="5" ht="26.25" customHeight="true">
@@ -5340,11 +5340,11 @@
       </c>
       <c r="C5" s="6" t="str">
         <f ca="1">IF(C3&lt;C2,ROUND(100*(C2-C3)/C2,0) &amp; "% Red",IF(C3=C2,0%,ROUND(100*(C3-C2)/C2,0) &amp; "% Inc"))</f>
-        <v>45% Red</v>
+        <v>38% Red</v>
       </c>
       <c r="D5" s="7" t="str">
         <f ca="1">IF(D3&lt;D2,ROUND(100*(D2-D3)/D2,0) &amp; "% Red",IF(D3=D2,0%,ROUND(100*(D3-D2)/D2,0) &amp; "% Inc"))</f>
-        <v>3% Red</v>
+        <v>1% Inc</v>
       </c>
     </row>
     <row r="7">
@@ -5943,7 +5943,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62">
@@ -5967,7 +5967,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65">
@@ -5975,7 +5975,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
@@ -7102,10 +7102,10 @@
         <v>23</v>
       </c>
       <c r="B29" s="14">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C29" s="14">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D29" s="16">
         <v>134.53</v>
@@ -7194,13 +7194,13 @@
         <v>19</v>
       </c>
       <c r="B33" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D33" s="16">
-        <v>60.51</v>
+        <v>0</v>
       </c>
       <c r="E33" s="3">
         <v>1</v>
@@ -7716,7 +7716,7 @@
       <c r="B63" s="33"/>
       <c r="C63" s="37"/>
       <c r="D63" s="38">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E63" s="5">
         <v>1</v>
@@ -7729,7 +7729,7 @@
       <c r="B64" s="33"/>
       <c r="C64" s="37"/>
       <c r="D64" s="38">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E64" s="5">
         <v>10</v>
@@ -7807,7 +7807,7 @@
       <c r="B70" s="33"/>
       <c r="C70" s="37"/>
       <c r="D70" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E70" s="5">
         <v>6</v>
@@ -8207,54 +8207,54 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A80:A91"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A92:A103"/>
+    <mergeCell ref="A40:B41"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="A61:C62"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A58:B58"/>
     <mergeCell ref="B78:B79"/>
-    <mergeCell ref="A80:A91"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A40:B41"/>
     <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A61:C62"/>
-    <mergeCell ref="A92:A103"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A76:C76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" scale="100" paperSize="9" fitToWidth="0" fitToHeight="0" horizontalDpi="0" verticalDpi="0" copies="1"/>
@@ -8880,9 +8880,9 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="H1:J1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H1:J1"/>
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
corrigiendo datos en afectaciones
</commit_message>
<xml_diff>
--- a/src/informesGenerados/ResumenFGR.xlsx
+++ b/src/informesGenerados/ResumenFGR.xlsx
@@ -8207,54 +8207,54 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A80:A91"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A45:B45"/>
     <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A92:A103"/>
-    <mergeCell ref="A40:B41"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A74:C74"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A40:B41"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A92:A103"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A61:C62"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="N1:R1"/>
     <mergeCell ref="A65:C65"/>
     <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A46:B46"/>
     <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="A61:C62"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A44:B44"/>
     <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A80:A91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" scale="100" paperSize="9" fitToWidth="0" fitToHeight="0" horizontalDpi="0" verticalDpi="0" copies="1"/>
@@ -8880,10 +8880,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" scale="100" paperSize="9" fitToWidth="0" fitToHeight="0" horizontalDpi="0" verticalDpi="0" copies="1"/>

</xml_diff>